<commit_message>
Section 3: Entering and Editing Text and Formulas Quiz
</commit_message>
<xml_diff>
--- a/Section 3: Entering and Editing Text and Formulas/Resources/monthlybudget.xlsx
+++ b/Section 3: Entering and Editing Text and Formulas/Resources/monthlybudget.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Desktop/excel/Section 3: Entering and Editing Text and Formulas/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 3: Entering and Editing Text and Formulas/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140F15E2-3568-E648-AA31-2F7806EC5AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C55FC6-ECC0-7547-9FFB-C0F8359A6A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{51F0C39A-75DD-F540-B849-5C49F44F8AE5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{51F0C39A-75DD-F540-B849-5C49F44F8AE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,8 +103,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65875596-FFE2-F64E-A595-6737C2AEB7A0}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,12 +430,12 @@
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -448,8 +451,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -462,8 +468,16 @@
       <c r="D4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f>B4+C4+D4</f>
+        <v>3000.55</v>
+      </c>
+      <c r="F4">
+        <f>E4/$E$9</f>
+        <v>0.58825086260978676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -476,8 +490,16 @@
       <c r="D5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f>B5+C5+D5</f>
+        <v>325.25</v>
+      </c>
+      <c r="F5">
+        <f>E5/$E$9</f>
+        <v>6.376450752823086E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -490,8 +512,16 @@
       <c r="D6">
         <v>175</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f>B6+C6+D6</f>
+        <v>525</v>
+      </c>
+      <c r="F6">
+        <f>E6/$E$9</f>
+        <v>0.10292503136762861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -504,8 +534,16 @@
       <c r="D7">
         <v>350</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f>B7+C7+D7</f>
+        <v>925</v>
+      </c>
+      <c r="F7">
+        <f>E7/$E$9</f>
+        <v>0.18134410288582181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -518,10 +556,38 @@
       <c r="D8">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f>B8+C8+D8</f>
+        <v>325</v>
+      </c>
+      <c r="F8">
+        <f>E8/$E$9</f>
+        <v>6.3715495608532E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9">
+        <f>B4+B5+B6+B7+B8</f>
+        <v>1650.8</v>
+      </c>
+      <c r="C9">
+        <f>C4+C5+C6+C7+C8</f>
+        <v>1700</v>
+      </c>
+      <c r="D9">
+        <f>D4+D5+D6+D7+D8</f>
+        <v>1750</v>
+      </c>
+      <c r="E9">
+        <f>B9+C9+D9</f>
+        <v>5100.8</v>
+      </c>
+      <c r="F9">
+        <f>E9/$E$9</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>